<commit_message>
만분율 float 변경, screen min,max 변경
</commit_message>
<xml_diff>
--- a/movement.xlsx
+++ b/movement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김주호\Documents\GitHub\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\endgame\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CCC2B1-A615-4E63-BD65-335648C8C2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54902308-B765-4C24-8575-FA58B5C2AB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{119698F5-A744-440C-A279-638743176699}"/>
+    <workbookView xWindow="1050" yWindow="540" windowWidth="25620" windowHeight="11385" xr2:uid="{119698F5-A744-440C-A279-638743176699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,10 @@
   </si>
   <si>
     <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,7 +525,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -570,7 +574,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>10</v>

</xml_diff>